<commit_message>
Add unique VINs to Each CA Select Test PT2 Add unique VINs to Each CA Choice Test, all
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New5VIN_CA_SELECT.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New5VIN_CA_SELECT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Desktop\SUITE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Documents\CSAA\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -224,7 +224,7 @@
     <t>SYMBOL_2000</t>
   </si>
   <si>
-    <t>EEENK3CC&amp;F</t>
+    <t>EEENK2CC&amp;F</t>
   </si>
 </sst>
 </file>
@@ -570,12 +570,12 @@
   <dimension ref="A1:AL5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" customWidth="1"/>

</xml_diff>